<commit_message>
resolve all the "quick fixes" issues and some of the "agreed actions" from stakeholder
</commit_message>
<xml_diff>
--- a/inst/app/www/FFT-QDC_Framework_MVP_version_20230925.xlsx
+++ b/inst/app/www/FFT-QDC_Framework_MVP_version_20230925.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30cf01616d186177/Documents/Local Githubs/experiencesdashboard/inst/app/www/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OMApe\OneDrive\Documents\Local Githubs\experiencesdashboard\inst\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="11_D98F16408C21DA5C6F08DB5C9810A6EC7902798A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC0B691F-3A8C-47DD-BC37-B386DD873A73}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53A2AE4-B4C0-44B8-8F08-EC2D33F65694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MVP framework" sheetId="1" r:id="rId1"/>
@@ -1112,9 +1112,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Comments relating to the extend to which patients are in physical pain, if and how pain relief is supplied, and whether pain is addressed in a timely and effective way in order to meet needs. </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Positive: </t>
     </r>
@@ -2005,6 +2002,9 @@
   </si>
   <si>
     <t>Did not answer', 'Feedback given', ' ' (i.e. blank text)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comments relating to the extent to which patients are in physical pain, if and how pain relief is supplied, and whether pain is addressed in a timely and effective way in order to meet needs. </t>
   </si>
 </sst>
 </file>
@@ -2668,8 +2668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2713,7 +2713,7 @@
       <c r="F4" s="32"/>
       <c r="G4" s="32"/>
     </row>
-    <row r="5" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="H7" s="30"/>
       <c r="I7" s="31"/>
     </row>
-    <row r="8" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
@@ -2830,7 +2830,7 @@
       </c>
       <c r="I13" s="31"/>
     </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>30</v>
       </c>
@@ -2863,7 +2863,7 @@
       <c r="H16" s="30"/>
       <c r="I16" s="31"/>
     </row>
-    <row r="17" spans="2:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
         <v>38</v>
       </c>
@@ -2906,8 +2906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBEE7D3-4ECA-48BB-A742-BFA7333E6BE7}">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2982,10 +2982,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2999,7 +2999,7 @@
         <v>54</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -3196,200 +3196,200 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
-        <v>27</v>
+    <row r="21" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C23" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="216" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:4" ht="216" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C25" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D27" s="19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>96</v>
+        <v>89</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="331.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="216" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B32" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C32" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="19" t="s">
+    </row>
+    <row r="33" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="19" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="19" t="s">
+      <c r="D33" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D30" s="19" t="s">
+      <c r="B34" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="19" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A31" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3398,6 +3398,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8fb53b4f-1204-4cd9-8a55-a9d7af4fbf3e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="cccaf3ac-2de9-44d4-aa31-54302fceb5f7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005FAB909D2035A345A9E4149139BE13AC" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="839134d19efc4c3ddedb863d6ac8a598">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="8fb53b4f-1204-4cd9-8a55-a9d7af4fbf3e" xmlns:ns3="9d2b163f-2795-4980-a00f-d619f53f7de8" xmlns:ns4="cccaf3ac-2de9-44d4-aa31-54302fceb5f7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4681ed9e497e539c7af53a4da4239c32" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3668,45 +3690,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8fb53b4f-1204-4cd9-8a55-a9d7af4fbf3e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="cccaf3ac-2de9-44d4-aa31-54302fceb5f7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{367A6B7F-254A-4B03-9A54-27973FD9EAA7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE12F67A-4B63-42E1-A654-2EE0AB95B353}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="8fb53b4f-1204-4cd9-8a55-a9d7af4fbf3e"/>
-    <ds:schemaRef ds:uri="9d2b163f-2795-4980-a00f-d619f53f7de8"/>
-    <ds:schemaRef ds:uri="cccaf3ac-2de9-44d4-aa31-54302fceb5f7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3731,9 +3718,22 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE12F67A-4B63-42E1-A654-2EE0AB95B353}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{367A6B7F-254A-4B03-9A54-27973FD9EAA7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="8fb53b4f-1204-4cd9-8a55-a9d7af4fbf3e"/>
+    <ds:schemaRef ds:uri="9d2b163f-2795-4980-a00f-d619f53f7de8"/>
+    <ds:schemaRef ds:uri="cccaf3ac-2de9-44d4-aa31-54302fceb5f7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>